<commit_message>
HMXBparamters heeft nu ook waarden voor: BC, B-V0, B-Vobs, mv, B, V, distance, Teff. Ook zijn de spectraaltypen nu van simbad gehaald voor alle objecten. En in tabledisplay wordt nu op basis van deze gegevens de luminosity berekend met de formules die staan in t logboek.
</commit_message>
<xml_diff>
--- a/HMXBkaper.xlsx
+++ b/HMXBkaper.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luukv\Documenten\NatuurSterrkenkundeMasterProject\CodeMP\MasterProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3AD40D3-BB4D-48A6-95E8-9FBDA3DC660A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D577C7-1230-4E56-B414-EEA2ED15B15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1230" windowWidth="29040" windowHeight="15840" xr2:uid="{050E6E13-3082-4035-A211-BD55BF94490B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{050E6E13-3082-4035-A211-BD55BF94490B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -38,6 +38,39 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
+    <t>B1 Ia</t>
+  </si>
+  <si>
+    <t>B0 Ib</t>
+  </si>
+  <si>
+    <t>O7 III-IV</t>
+  </si>
+  <si>
+    <t>B0.5 Ib</t>
+  </si>
+  <si>
+    <t>O6.5 II-III</t>
+  </si>
+  <si>
+    <t>B1.5 Ia+</t>
+  </si>
+  <si>
+    <t>B0 Iab</t>
+  </si>
+  <si>
+    <t>O6.5 Iaf+</t>
+  </si>
+  <si>
+    <t>early B I</t>
+  </si>
+  <si>
+    <t>O7-9 III</t>
+  </si>
+  <si>
+    <t>O9.7 Iab</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -83,70 +116,37 @@
     <t>luminosity</t>
   </si>
   <si>
-    <t>2S0114+650</t>
-  </si>
-  <si>
-    <t>SMC X-1</t>
-  </si>
-  <si>
-    <t>LMC X-4</t>
-  </si>
-  <si>
-    <t>Vela X-1</t>
-  </si>
-  <si>
-    <t>Cen X-3</t>
-  </si>
-  <si>
-    <t>GX301-2</t>
-  </si>
-  <si>
-    <t>4U1538-52</t>
-  </si>
-  <si>
-    <t>4U1700-37</t>
-  </si>
-  <si>
-    <t>4U1907+09</t>
-  </si>
-  <si>
-    <t>LMC X-1</t>
-  </si>
-  <si>
-    <t>Cyg X-1</t>
-  </si>
-  <si>
-    <t>B1 Ia</t>
-  </si>
-  <si>
-    <t>B0 Ib</t>
-  </si>
-  <si>
-    <t>O7 III-IV</t>
-  </si>
-  <si>
-    <t>B0.5 Ib</t>
-  </si>
-  <si>
-    <t>O6.5 II-III</t>
-  </si>
-  <si>
-    <t>B1.5 Ia+</t>
-  </si>
-  <si>
-    <t>B0 Iab</t>
-  </si>
-  <si>
-    <t>O6.5 Iaf+</t>
-  </si>
-  <si>
-    <t>early B I</t>
-  </si>
-  <si>
-    <t>O7-9 III</t>
-  </si>
-  <si>
-    <t>O9.7 Iab</t>
+    <t>2S0114+650(K)</t>
+  </si>
+  <si>
+    <t>SMC X-1(K)</t>
+  </si>
+  <si>
+    <t>LMC X-4(K)</t>
+  </si>
+  <si>
+    <t>Vela X-1(K)</t>
+  </si>
+  <si>
+    <t>Cen X-3(K)</t>
+  </si>
+  <si>
+    <t>GX301-2(K)</t>
+  </si>
+  <si>
+    <t>4U1538-52(K)</t>
+  </si>
+  <si>
+    <t>4U1700-37(K)</t>
+  </si>
+  <si>
+    <t>4U1907+09(K)</t>
+  </si>
+  <si>
+    <t>LMC X-1(K)</t>
+  </si>
+  <si>
+    <t>Cyg X-1(K)</t>
   </si>
 </sst>
 </file>
@@ -510,74 +510,73 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
-    <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
       </c>
       <c r="E2">
         <v>860</v>
@@ -592,12 +591,12 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0.71</v>
@@ -612,12 +611,12 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>13.5</v>
@@ -632,12 +631,12 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="E5">
         <v>283</v>
@@ -655,12 +654,12 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="E6">
         <v>4.84</v>
@@ -678,12 +677,12 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <v>696</v>
@@ -698,12 +697,12 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="E8">
         <v>529</v>
@@ -721,12 +720,12 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="G9">
         <v>76</v>
@@ -741,12 +740,12 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="E10">
         <v>438</v>
@@ -758,23 +757,23 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="J11">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="G12">
         <v>20</v>

</xml_diff>